<commit_message>
update expected result to use releative path
</commit_message>
<xml_diff>
--- a/SeleniumPythonFramework/src/TestPlan/Plan1.xlsx
+++ b/SeleniumPythonFramework/src/TestPlan/Plan1.xlsx
@@ -429,12 +429,12 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>01-22 12:49:30</t>
+          <t>01-30 21:57:51</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>01-22 12:49:38</t>
+          <t>01-30 21:57:59</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">

</xml_diff>